<commit_message>
minor edits to Part III of thesis, updated some data files
</commit_message>
<xml_diff>
--- a/Management/Thesis Schedule.xlsx
+++ b/Management/Thesis Schedule.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="26">
   <si>
     <t>October</t>
   </si>
@@ -87,24 +87,29 @@
     <t>curve-fitting and other software development</t>
   </si>
   <si>
-    <t>target selection automation</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>draft of first chapter done (12.411 final report)</t>
-  </si>
-  <si>
     <t>initial presentations</t>
+  </si>
+  <si>
+    <t>introduction and background section draft</t>
+  </si>
+  <si>
+    <t>curve-fitting chapter and appendix</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -258,7 +263,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
@@ -271,13 +276,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -585,7 +592,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,18 +603,18 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="11"/>
-      <c r="B1" s="12">
+      <c r="B1" s="13">
         <v>2013</v>
       </c>
-      <c r="C1" s="12"/>
-      <c r="D1" s="12"/>
-      <c r="E1" s="12">
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13">
         <v>2014</v>
       </c>
-      <c r="F1" s="12"/>
-      <c r="G1" s="12"/>
-      <c r="H1" s="12"/>
-      <c r="I1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="14"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
@@ -669,18 +676,18 @@
       <c r="B5" s="4"/>
       <c r="C5" s="6"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="4"/>
+      <c r="E5" s="6"/>
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="5"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="16" t="s">
         <v>11</v>
       </c>
       <c r="B6" s="4"/>
-      <c r="C6" s="6"/>
+      <c r="C6" s="4"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -689,12 +696,12 @@
       <c r="I6" s="5"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>22</v>
+      <c r="A7" s="15" t="s">
+        <v>24</v>
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="6"/>
+      <c r="D7" s="4"/>
       <c r="E7" s="6"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
@@ -702,15 +709,13 @@
       <c r="I7" s="5"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>23</v>
+      <c r="A8" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="4"/>
       <c r="G8" s="4"/>
       <c r="H8" s="4"/>
@@ -730,7 +735,7 @@
       <c r="I9" s="5"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="16" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="4"/>
@@ -758,8 +763,8 @@
       <c r="I11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>26</v>
+      <c r="A12" s="12" t="s">
+        <v>23</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>

</xml_diff>